<commit_message>
Avance historia de usaurio registro, criterios de aceptación
</commit_message>
<xml_diff>
--- a/hus/HU-IW-001 -Registro.xlsx
+++ b/hus/HU-IW-001 -Registro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\universidad\ingewev\turismo\hus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950A521B-98D6-4EE5-8FEA-83E6A7F892DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA2DF71-B798-4DEB-B822-ADBEFBB2DE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>Proyecto</t>
   </si>
@@ -116,39 +116,6 @@
     <t>Revision de la redacción</t>
   </si>
   <si>
-    <t>Dado que el coordinador esta en la gestión de expedientes</t>
-  </si>
-  <si>
-    <t>Cuando pulse el boton consultar</t>
-  </si>
-  <si>
-    <t>se debe listar los expedientes cargados con la marca "validado por geomática"</t>
-  </si>
-  <si>
-    <t>Escenario 2: Cualificación de expediente</t>
-  </si>
-  <si>
-    <t>cuando pulse el boton detalles</t>
-  </si>
-  <si>
-    <t>Se debe indicar si el el expediente esta: 0 -&gt; esta fuera, 1-&gt; esta dentro, 2 -&gt; no encontrado.</t>
-  </si>
-  <si>
-    <t>Escenario 1: Validación de carga</t>
-  </si>
-  <si>
-    <t>Escenario 1: Carga de expedientes</t>
-  </si>
-  <si>
-    <t>Dado que el coordinador dispone de esta funcionalidad</t>
-  </si>
-  <si>
-    <t>Cuando seleccione el archivo DBF y pulse el botón "Cargar"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema debe confirmar el número de registros cargados </t>
-  </si>
-  <si>
     <t>Actor</t>
   </si>
   <si>
@@ -231,6 +198,27 @@
   </si>
   <si>
     <t>cualquiera</t>
+  </si>
+  <si>
+    <t>1. Campos requeridos</t>
+  </si>
+  <si>
+    <t>Dado que el usuario esta llenando el formlario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cuando haya omitido campos sin llenar </t>
+  </si>
+  <si>
+    <t>se le deben marcar todos los campos que le faltan por diligenciar y el botón de registro no se debe habilitar</t>
+  </si>
+  <si>
+    <t>2. Usuario existente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cuando envíe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dado que el usuario ingreso un </t>
   </si>
 </sst>
 </file>
@@ -540,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -597,6 +585,53 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -605,62 +640,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -981,8 +972,8 @@
   </sheetPr>
   <dimension ref="A1:G998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1013,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1040,343 +1031,333 @@
     </row>
     <row r="5" spans="1:7" ht="14.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" ht="14.4">
       <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
+      <c r="C6" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" ht="28.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
+      <c r="C7" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
+      <c r="C9" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:7" ht="14.4">
       <c r="A10" s="1"/>
-      <c r="B10" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
+      <c r="B10" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" ht="14.4">
       <c r="A11" s="1"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:7" ht="14.4">
       <c r="A12" s="1"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="53"/>
-      <c r="C14" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="54"/>
+      <c r="C14" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="53"/>
-      <c r="C15" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="54">
+      <c r="C15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="28">
         <v>80</v>
       </c>
-      <c r="G15" s="54"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" ht="34.200000000000003" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="53"/>
-      <c r="C16" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-    </row>
-    <row r="17" spans="1:7" ht="43.2">
+      <c r="C16" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" ht="28.8">
       <c r="A17" s="1"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" ht="43.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="54" t="s">
+      <c r="B18" s="54"/>
+      <c r="C18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7" ht="43.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" ht="14.4">
       <c r="A20" s="1"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="54" t="s">
+      <c r="B20" s="54"/>
+      <c r="C20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="E20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="1:7" ht="43.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" spans="1:7" ht="14.4">
       <c r="A22" s="1"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" spans="1:7" ht="14.4">
       <c r="A23" s="1"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="14.4">
       <c r="A24" s="1"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="46"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="41.4">
       <c r="A26" s="1"/>
-      <c r="B26" s="41"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="25" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="52"/>
+        <v>56</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="48"/>
       <c r="G26" s="26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="41.4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="27.6">
       <c r="A27" s="1"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="48"/>
-      <c r="G27" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="42">
+      <c r="B27" s="35"/>
+      <c r="C27" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="44"/>
+      <c r="G27" s="23"/>
+    </row>
+    <row r="28" spans="1:7" ht="14.4">
       <c r="A28" s="1"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="50"/>
-      <c r="G28" s="24" t="s">
-        <v>32</v>
-      </c>
+      <c r="B28" s="35"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7" ht="14.4">
       <c r="A29" s="1"/>
-      <c r="B29" s="39"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="33"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" ht="14.4">
@@ -1393,18 +1374,18 @@
     </row>
     <row r="32" spans="1:7" ht="14.4">
       <c r="A32" s="1"/>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="14.4">
       <c r="A33" s="1"/>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="37" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -1425,7 +1406,7 @@
     </row>
     <row r="34" spans="1:7" ht="16.5" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="36"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -1434,7 +1415,7 @@
     </row>
     <row r="35" spans="1:7" ht="14.4">
       <c r="A35" s="1"/>
-      <c r="B35" s="36"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="13"/>
       <c r="D35" s="14"/>
       <c r="E35" s="15"/>
@@ -1443,7 +1424,7 @@
     </row>
     <row r="36" spans="1:7" ht="14.4">
       <c r="A36" s="1"/>
-      <c r="B36" s="44"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
@@ -1452,7 +1433,7 @@
     </row>
     <row r="37" spans="1:7" ht="28.2">
       <c r="A37" s="1"/>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="9" t="s">
@@ -1471,7 +1452,7 @@
     </row>
     <row r="38" spans="1:7" ht="32.25" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="36"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="11"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10" t="s">
@@ -1484,7 +1465,7 @@
     </row>
     <row r="39" spans="1:7" ht="14.4">
       <c r="A39" s="1"/>
-      <c r="B39" s="36"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="11"/>
       <c r="D39" s="10"/>
       <c r="E39" s="18">
@@ -1497,7 +1478,7 @@
     </row>
     <row r="40" spans="1:7" ht="14.4">
       <c r="A40" s="1"/>
-      <c r="B40" s="36"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="19"/>
       <c r="D40" s="20"/>
       <c r="E40" s="21"/>
@@ -1506,7 +1487,7 @@
     </row>
     <row r="41" spans="1:7" ht="14.4">
       <c r="A41" s="1"/>
-      <c r="B41" s="39"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
@@ -2488,15 +2469,6 @@
     <row r="998" ht="14.4"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E26:F26"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="B13:B24"/>
@@ -2508,6 +2480,15 @@
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C10:G10"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se suben historias de usuario de login y compra y formularios en html
</commit_message>
<xml_diff>
--- a/hus/HU-IW-001 -Registro.xlsx
+++ b/hus/HU-IW-001 -Registro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\universidad\ingewev\turismo\hus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA2DF71-B798-4DEB-B822-ADBEFBB2DE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62425EF8-B2B6-4E4C-A52F-ED0F5A2BCBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Proyecto</t>
   </si>
@@ -215,10 +215,53 @@
     <t>2. Usuario existente</t>
   </si>
   <si>
-    <t xml:space="preserve">cuando envíe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dado que el usuario ingreso un </t>
+    <t>cuando el usuario haga click en registrar</t>
+  </si>
+  <si>
+    <t>El sistema le debe informar en una ventana modal que ya existe en la base de datos.</t>
+  </si>
+  <si>
+    <t>Dado que el usuario ingreso una cédula, o un correo existente</t>
+  </si>
+  <si>
+    <t>3. Usuario creado exitósamente</t>
+  </si>
+  <si>
+    <t>Dado que el usuario ingresó la información de manera correcta</t>
+  </si>
+  <si>
+    <t>Cuando el usuario se cree satisfactoriamente en la base de datos</t>
+  </si>
+  <si>
+    <t>Se debe cerrar automáticamente el formulario de creación y redirigir al formulario de login</t>
+  </si>
+  <si>
+    <t>4. Contraseña debil</t>
+  </si>
+  <si>
+    <t>El usuario ingreso una contraseña que no concuerda con el siguiente patrón</t>
+  </si>
+  <si>
+    <t>5. Correo inválido</t>
+  </si>
+  <si>
+    <t>Dado que el usuario ha ingresado un correo que no cumple con el formato</t>
+  </si>
+  <si>
+    <t>Cuando abandone el campo</t>
+  </si>
+  <si>
+    <t>Entonces el campo se debe marcar en rojo y mostrar un texto debajo del campo diciendo que no es un correo válido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando el usurio digite en el campo </t>
+  </si>
+  <si>
+    <t>Se debe marcar el campo en rojo, en rojo cual de los siguientos requisitos no ha cumplido
+-Mínimo 8 caracteres
+-Mínimo un número
+-Mínimo un simbolo
+-Mínimo una letra en mayúsuculas y una en minúsculas</t>
   </si>
 </sst>
 </file>
@@ -228,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -286,6 +329,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -528,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -541,10 +597,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -590,8 +642,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -601,6 +653,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -609,28 +662,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -650,8 +699,21 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -970,10 +1032,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G998"/>
+  <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1031,488 +1093,522 @@
     </row>
     <row r="5" spans="1:7" ht="14.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="32"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="14.4">
       <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="32"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7" ht="28.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="32"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="32"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="32"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7" ht="14.4">
       <c r="A10" s="1"/>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="32"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:7" ht="14.4">
       <c r="A11" s="1"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:7" ht="14.4">
       <c r="A12" s="1"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="32"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="29" t="s">
+      <c r="B14" s="50"/>
+      <c r="C14" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="50"/>
+      <c r="C15" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="26">
         <v>80</v>
       </c>
-      <c r="G15" s="28"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7" ht="34.200000000000003" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="28" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7" ht="28.8">
       <c r="A17" s="1"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" ht="43.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" ht="43.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="28" t="s">
+      <c r="B19" s="51"/>
+      <c r="C19" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" ht="14.4">
       <c r="A20" s="1"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="28" t="s">
+      <c r="B20" s="51"/>
+      <c r="C20" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" ht="43.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="28" t="s">
+      <c r="B21" s="51"/>
+      <c r="C21" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" ht="14.4">
       <c r="A22" s="1"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="28" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:7" ht="14.4">
       <c r="A23" s="1"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" ht="14.4">
       <c r="A24" s="1"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="31" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="41" t="s">
+      <c r="E25" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="42"/>
+      <c r="F25" s="40"/>
       <c r="G25" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="41.4">
       <c r="A26" s="1"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="25" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="26" t="s">
+      <c r="F26" s="44"/>
+      <c r="G26" s="24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="27.6">
+    <row r="27" spans="1:7" ht="41.4">
       <c r="A27" s="1"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="57" t="s">
+      <c r="B27" s="33"/>
+      <c r="C27" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="42"/>
+      <c r="G27" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="44"/>
-      <c r="G27" s="23"/>
-    </row>
-    <row r="28" spans="1:7" ht="14.4">
+    </row>
+    <row r="28" spans="1:7" ht="41.4">
       <c r="A28" s="1"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="24"/>
-    </row>
-    <row r="29" spans="1:7" ht="14.4">
+      <c r="B28" s="34"/>
+      <c r="C28" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="45"/>
+      <c r="G28" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="111">
       <c r="A29" s="1"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" ht="14.4">
+      <c r="B29" s="33"/>
+      <c r="C29" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="59"/>
+      <c r="G29" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="55.8">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="30"/>
+      <c r="G30" s="56" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="14.4">
       <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="14.4">
       <c r="A32" s="1"/>
-      <c r="B32" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="14.4">
       <c r="A33" s="1"/>
       <c r="B33" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="30"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C34" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A34" s="1"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="12"/>
-    </row>
-    <row r="35" spans="1:7" ht="14.4">
+    <row r="35" spans="1:7" ht="16.5" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" ht="14.4">
       <c r="A36" s="1"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="12"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="12"/>
-    </row>
-    <row r="37" spans="1:7" ht="28.2">
+      <c r="E36" s="13"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" ht="14.4">
       <c r="A37" s="1"/>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="34"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" ht="28.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E38" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="17"/>
-    </row>
-    <row r="38" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A38" s="1"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10" t="s">
+      <c r="G38" s="15"/>
+    </row>
+    <row r="39" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A39" s="1"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="10" t="s">
+      <c r="F39" s="10"/>
+      <c r="G39" s="8" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="14.4">
-      <c r="A39" s="1"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="18">
-        <v>42370</v>
-      </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14.4">
       <c r="A40" s="1"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="16">
+        <v>42370</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="14.4">
       <c r="A41" s="1"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" ht="14.4">
       <c r="A42" s="1"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" ht="14.4">
       <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="14.4"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+    </row>
+    <row r="44" spans="1:7" ht="14.4">
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
     <row r="45" spans="1:7" ht="14.4"/>
     <row r="46" spans="1:7" ht="14.4"/>
     <row r="47" spans="1:7" ht="14.4"/>
@@ -2467,8 +2563,9 @@
     <row r="996" ht="14.4"/>
     <row r="997" ht="14.4"/>
     <row r="998" ht="14.4"/>
+    <row r="999" ht="14.4"/>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="B13:B24"/>
@@ -2480,15 +2577,16 @@
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C10:G10"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:B37"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E26:F26"/>
     <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>